<commit_message>
new file:   .idea/vcs.xml 	modified:   etap_to_excel.py 	modified:   parameters.xlsx
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -10,6 +10,9 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="INVERTER" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DCLUMPLOAD" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BATTERY" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DCCABLE" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DCBUS" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DC_IMPEDANCE" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -428,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,115 +452,125 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>InService</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>STATE</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Felement</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Telement</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>ACkV</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>DCV</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>KVA</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>DCKW</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>DCEff</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Vref</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Smax</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Pmax</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Qmax</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>generate_V1</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>generate_V2</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>generate_V3</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>generate_P1</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>generate_P2</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>generate_P3</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>charge_V1</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>charge_V2</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>charge_V3</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>charge_P1</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>charge_P2</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>charge_P3</t>
         </is>
@@ -574,115 +587,125 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>Bus2</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>dcBus1</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>0.400000006</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>824</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>135</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>150</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>90</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>100</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>135</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>135</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>135</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>88.00</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>106.00</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>110.00</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>100.00</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>100.00</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>20.00</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="V2" t="inlineStr">
         <is>
           <t>88.00</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="W2" t="inlineStr">
         <is>
           <t>106.00</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="X2" t="inlineStr">
         <is>
           <t>110.00</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
+      <c r="Y2" t="inlineStr">
         <is>
           <t>20.00</t>
         </is>
       </c>
-      <c r="X2" t="inlineStr">
+      <c r="Z2" t="inlineStr">
         <is>
           <t>20.00</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr">
+      <c r="AA2" t="inlineStr">
         <is>
           <t>20.00</t>
         </is>
@@ -697,18 +720,18 @@
           <t>Inv2</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
           <t>0</t>
@@ -721,24 +744,24 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
           <t>90</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>100</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="M3" t="inlineStr">
         <is>
           <t>0</t>
@@ -746,60 +769,70 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
           <t>88.00</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>106.00</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="R3" t="inlineStr">
         <is>
           <t>110.00</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="S3" t="inlineStr">
         <is>
           <t>100.00</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>100.00</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="U3" t="inlineStr">
         <is>
           <t>20.00</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="V3" t="inlineStr">
         <is>
           <t>88.00</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="W3" t="inlineStr">
         <is>
           <t>106.00</t>
         </is>
       </c>
-      <c r="V3" t="inlineStr">
+      <c r="X3" t="inlineStr">
         <is>
           <t>110.00</t>
         </is>
       </c>
-      <c r="W3" t="inlineStr">
+      <c r="Y3" t="inlineStr">
         <is>
           <t>10.00</t>
         </is>
       </c>
-      <c r="X3" t="inlineStr">
+      <c r="Z3" t="inlineStr">
         <is>
           <t>10.00</t>
         </is>
       </c>
-      <c r="Y3" t="inlineStr">
+      <c r="AA3" t="inlineStr">
         <is>
           <t>20.00</t>
         </is>
@@ -814,18 +847,18 @@
           <t>Inv3</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
           <t>0</t>
@@ -838,24 +871,24 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
           <t>90</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>100</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="M4" t="inlineStr">
         <is>
           <t>0</t>
@@ -863,60 +896,70 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="R4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="S4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="U4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="T4" t="inlineStr">
+      <c r="V4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="U4" t="inlineStr">
+      <c r="W4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="V4" t="inlineStr">
+      <c r="X4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="W4" t="inlineStr">
+      <c r="Y4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="X4" t="inlineStr">
+      <c r="Z4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="Y4" t="inlineStr">
+      <c r="AA4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
@@ -933,7 +976,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -954,15 +997,25 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>InService</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>STATE</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>BUS_I</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>RatedV</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>RatedKW</t>
         </is>
@@ -979,15 +1032,25 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>dcBus1</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>824</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -1004,15 +1067,25 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>dcBus6</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>824</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -1027,13 +1100,23 @@
           <t>dcLump2</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>824</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -1048,13 +1131,23 @@
           <t>dcLump3</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>824</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -1069,13 +1162,23 @@
           <t>dcLump4</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>824</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -1092,7 +1195,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1113,20 +1216,30 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>InService</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>STATE</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>BusID</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Cells</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Packs</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Strings</t>
         </is>
@@ -1143,20 +1256,30 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>dcBus3</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>20</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>20</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>20</t>
         </is>
@@ -1171,18 +1294,28 @@
           <t>Battery3</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>20</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>20</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>20</t>
         </is>
@@ -1197,20 +1330,679 @@
           <t>Battery2</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>20</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>IID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>STATE</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>FromBus</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ToBus</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>LENGTH</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>LENGTH_Unit</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>OhmsPerLengthValue</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>OhmsPerLengthUnit</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>RPosValue</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>XPosValue</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>DC Cable1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>IID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>NominalV</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>STATE</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>dcBus1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>824</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>dcBus3</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>824</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>dcBus8</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>824</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>As-Built</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>dcBus5</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>824</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>dcBus6</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>824</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>dcBus2</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>dcBus4</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>824</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>dcBus7</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>824</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>dcBus9</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>IID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>STATE</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>FromBus</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ToBus</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>RValue</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>LValue</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>dcZ1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>dcBus3</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>dcBus1</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.200000003</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>dcZ5</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>dcBus5</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>dcBus8</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.00400000019</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>dcZ3</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>dcBus6</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>dcBus5</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0.200000003</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>dcZ2</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.200000003</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>dcZ4</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>As-Built</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>0.200000003</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
modified:   README.md 	modified:   etap_to_excel.py 	modified:   parameters.xlsx 	new file:   ~$parameters.xlsx
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA4"/>
+  <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,80 +497,90 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>ACkW</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>ACkVar</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>Vref</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Smax</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Pmax</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Qmax</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>generate_V1</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>generate_V2</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>generate_V3</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>generate_P1</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>generate_P2</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>generate_P3</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>charge_V1</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>charge_V2</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>charge_V3</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>charge_P1</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>charge_P2</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>charge_P3</t>
         </is>
@@ -637,75 +647,85 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
           <t>135</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>135</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>135</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>88.00</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>106.00</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>110.00</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>100.00</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="V2" t="inlineStr">
         <is>
           <t>100.00</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="W2" t="inlineStr">
         <is>
           <t>20.00</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="X2" t="inlineStr">
         <is>
           <t>88.00</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
+      <c r="Y2" t="inlineStr">
         <is>
           <t>106.00</t>
         </is>
       </c>
-      <c r="X2" t="inlineStr">
+      <c r="Z2" t="inlineStr">
         <is>
           <t>110.00</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr">
+      <c r="AA2" t="inlineStr">
         <is>
           <t>20.00</t>
         </is>
       </c>
-      <c r="Z2" t="inlineStr">
+      <c r="AB2" t="inlineStr">
         <is>
           <t>20.00</t>
         </is>
       </c>
-      <c r="AA2" t="inlineStr">
+      <c r="AC2" t="inlineStr">
         <is>
           <t>20.00</t>
         </is>
@@ -759,19 +779,19 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
           <t>100</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="O3" t="inlineStr">
         <is>
           <t>0</t>
@@ -779,60 +799,70 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
           <t>88.00</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="S3" t="inlineStr">
         <is>
           <t>106.00</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>110.00</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="U3" t="inlineStr">
         <is>
           <t>100.00</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="V3" t="inlineStr">
         <is>
           <t>100.00</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="W3" t="inlineStr">
         <is>
           <t>20.00</t>
         </is>
       </c>
-      <c r="V3" t="inlineStr">
+      <c r="X3" t="inlineStr">
         <is>
           <t>88.00</t>
         </is>
       </c>
-      <c r="W3" t="inlineStr">
+      <c r="Y3" t="inlineStr">
         <is>
           <t>106.00</t>
         </is>
       </c>
-      <c r="X3" t="inlineStr">
+      <c r="Z3" t="inlineStr">
         <is>
           <t>110.00</t>
         </is>
       </c>
-      <c r="Y3" t="inlineStr">
+      <c r="AA3" t="inlineStr">
         <is>
           <t>10.00</t>
         </is>
       </c>
-      <c r="Z3" t="inlineStr">
+      <c r="AB3" t="inlineStr">
         <is>
           <t>10.00</t>
         </is>
       </c>
-      <c r="AA3" t="inlineStr">
+      <c r="AC3" t="inlineStr">
         <is>
           <t>20.00</t>
         </is>
@@ -886,19 +916,19 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
           <t>100</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="O4" t="inlineStr">
         <is>
           <t>0</t>
@@ -906,60 +936,70 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="S4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="U4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="T4" t="inlineStr">
+      <c r="V4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="U4" t="inlineStr">
+      <c r="W4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="V4" t="inlineStr">
+      <c r="X4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="W4" t="inlineStr">
+      <c r="Y4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="X4" t="inlineStr">
+      <c r="Z4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="Y4" t="inlineStr">
+      <c r="AA4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="Z4" t="inlineStr">
+      <c r="AB4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="AA4" t="inlineStr">
+      <c r="AC4" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>

</xml_diff>